<commit_message>
Organize and compile Vintage 2009 components of change data in stata.
</commit_message>
<xml_diff>
--- a/excel_analysis/population_growth.xlsx
+++ b/excel_analysis/population_growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/elizabethbageant_uidaho_edu/Documents/MAIN/Projects/Growth in Idaho 2024/Pop_Change_Analysis4/excel_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{FB04E5D8-01AF-674C-AAA2-D64FA078AEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4511D850-6018-FC49-B179-938502DC0E94}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{FB04E5D8-01AF-674C-AAA2-D64FA078AEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF841533-F852-F245-A3BE-61306A40A167}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{6B66F476-AA26-DD4B-A27D-A91A8A8ED334}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Idaho population</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual population growth: </t>
+    <t xml:space="preserve">Annual population growth from 2014-2023: </t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>